<commit_message>
centered models of m5 m6, penalpoint confirmed, but confirming prisonhelp and prisonpen
</commit_message>
<xml_diff>
--- a/real_raw_codebook.xlsx
+++ b/real_raw_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinamensik/Documents/Duke/2024-2025/902 Legislators Pre-Ananlysis Plan/Prelim Folder/Prelim 3-23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinamensik/Documents/GitHub/phd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9A889F-6385-B34C-95F7-998BAEA35091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC29FDAF-3EC2-CC48-A69C-B84FFCB6B4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11140" yWindow="500" windowWidth="21540" windowHeight="20640" xr2:uid="{6DE5729F-1ACE-E84F-B695-E91F62472D2C}"/>
+    <workbookView xWindow="48300" yWindow="500" windowWidth="38140" windowHeight="19620" xr2:uid="{6DE5729F-1ACE-E84F-B695-E91F62472D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5190,8 +5190,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5528,8 +5531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94F1213-98D1-E742-8DD0-94E9E254DC20}">
   <dimension ref="A1:D572"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A404" workbookViewId="0">
+      <selection activeCell="C428" sqref="C428"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11517,14 +11520,14 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>1236</v>
       </c>
       <c r="B428" t="s">
         <v>1677</v>
       </c>
-      <c r="C428" t="s">
+      <c r="C428" s="1" t="s">
         <v>1237</v>
       </c>
       <c r="D428" t="s">

</xml_diff>

<commit_message>
variance and starting to look at by impact
</commit_message>
<xml_diff>
--- a/real_raw_codebook.xlsx
+++ b/real_raw_codebook.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinamensik/Documents/GitHub/phd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC29FDAF-3EC2-CC48-A69C-B84FFCB6B4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE2FBED-860B-3946-B2C2-492CEC9A05EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48300" yWindow="500" windowWidth="38140" windowHeight="19620" xr2:uid="{6DE5729F-1ACE-E84F-B695-E91F62472D2C}"/>
+    <workbookView xWindow="51220" yWindow="980" windowWidth="31160" windowHeight="19620" xr2:uid="{6DE5729F-1ACE-E84F-B695-E91F62472D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -5531,8 +5531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94F1213-98D1-E742-8DD0-94E9E254DC20}">
   <dimension ref="A1:D572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A404" workbookViewId="0">
-      <selection activeCell="C428" sqref="C428"/>
+    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="C315" sqref="C315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>